<commit_message>
Added solutions to some descriptive statistics exercises.
</commit_message>
<xml_diff>
--- a/descriptive_statistics/grades-gender.xlsx
+++ b/descriptive_statistics/grades-gender.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="6210"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="19440" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,8 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -290,6 +290,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -372,11 +373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="39115392"/>
-        <c:axId val="106951424"/>
+        <c:axId val="71241728"/>
+        <c:axId val="71244032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39115392"/>
+        <c:axId val="71241728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,13 +399,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106951424"/>
+        <c:crossAx val="71244032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -412,7 +414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106951424"/>
+        <c:axId val="71244032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,13 +436,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39115392"/>
+        <c:crossAx val="71241728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -471,7 +474,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[grades-sex.xlsx]Solution-3-4!PivotTable5</c:name>
+    <c:name>[grades-gender.xlsx]Solution-3-4!PivotTable5</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -720,11 +723,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="108595840"/>
-        <c:axId val="108606208"/>
+        <c:axId val="77669504"/>
+        <c:axId val="77671424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108595840"/>
+        <c:axId val="77669504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,12 +749,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108606208"/>
+        <c:crossAx val="77671424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108606208"/>
+        <c:axId val="77671424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,19 +786,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108595840"/>
+        <c:crossAx val="77669504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -834,7 +840,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[grades-sex.xlsx]Solution-3-4!PivotTable5</c:name>
+    <c:name>[grades-gender.xlsx]Solution-3-4!PivotTable5</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -1067,11 +1073,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="108632320"/>
-        <c:axId val="108642688"/>
+        <c:axId val="83119488"/>
+        <c:axId val="84286080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108632320"/>
+        <c:axId val="83119488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,12 +1099,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108642688"/>
+        <c:crossAx val="84286080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1106,7 +1113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108642688"/>
+        <c:axId val="84286080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,19 +1139,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108632320"/>
+        <c:crossAx val="83119488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1184,7 +1193,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[grades-sex.xlsx]Solution-5!PivotTable7</c:name>
+    <c:name>[grades-gender.xlsx]Solution-5!PivotTable7</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -1209,6 +1218,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1336,11 +1346,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="108795008"/>
-        <c:axId val="108796928"/>
+        <c:axId val="79745408"/>
+        <c:axId val="79747328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108795008"/>
+        <c:axId val="79745408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,12 +1372,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108796928"/>
+        <c:crossAx val="79747328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1375,7 +1386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108796928"/>
+        <c:axId val="79747328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,13 +1408,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108795008"/>
+        <c:crossAx val="79745408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1444,7 +1456,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[grades-sex.xlsx]Solution-5!PivotTable6</c:name>
+    <c:name>[grades-gender.xlsx]Solution-5!PivotTable6</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1464,6 +1476,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1597,11 +1610,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="108832256"/>
-        <c:axId val="108834176"/>
+        <c:axId val="82258560"/>
+        <c:axId val="82264832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108832256"/>
+        <c:axId val="82258560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,12 +1636,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108834176"/>
+        <c:crossAx val="82264832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1636,7 +1650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108834176"/>
+        <c:axId val="82264832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,13 +1672,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108832256"/>
+        <c:crossAx val="82258560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6117,7 +6132,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G3:H13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="2">
     <pivotField axis="axisPage" showAll="0">
@@ -6204,7 +6219,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="2">
     <pivotField axis="axisPage" dataField="1" showAll="0">
@@ -6308,7 +6323,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" showAll="0">
@@ -6448,7 +6463,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="2">
     <pivotField axis="axisPage" dataField="1" showAll="0">
@@ -6570,7 +6585,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D3:E13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="2">
     <pivotField axis="axisPage" showAll="0">
@@ -15112,7 +15127,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:XFD1048576"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15520,8 +15535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15705,7 +15720,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>